<commit_message>
bat was create execurable, fixed because of I excluded some packages
</commit_message>
<xml_diff>
--- a/sitemaps.xlsx
+++ b/sitemaps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caglar.sarikaya\Desktop\test-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caglar.sarikaya\Documents\GitHub\url-tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2C9C2B-E6C2-4EED-A22E-4B422E260F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686DBB25-184D-4797-8456-6200259D5DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1110" yWindow="2040" windowWidth="21600" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,25 +20,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>sitemap_url</t>
   </si>
   <si>
     <t>root</t>
   </si>
-  <si>
-    <t>https://www.ntv.com.tr/proverbs-sitemap</t>
-  </si>
-  <si>
-    <t>https://www.ntv.com.tr</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,14 +51,6 @@
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="162"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,20 +85,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,15 +396,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -433,21 +417,9 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A2" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{C7113C31-5952-43F2-B493-873B7C643FD5}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{5DBC5D81-CA6A-44BC-8758-D402064F3F70}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
concurrent thread adjustable, it was getting timeouts with 100 threads
</commit_message>
<xml_diff>
--- a/sitemaps.xlsx
+++ b/sitemaps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caglar.sarikaya\Documents\GitHub\url-tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686DBB25-184D-4797-8456-6200259D5DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5499C0FF-6F9A-48C8-A2FA-DEA7D9D54975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1110" yWindow="2040" windowWidth="21600" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,13 +44,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="162"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,12 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,9 +408,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>